<commit_message>
Improved analysis logic, added logic to loop through multiple worksheets
</commit_message>
<xml_diff>
--- a/expenses.xlsx
+++ b/expenses.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="208">
   <si>
     <t>Expense</t>
   </si>
@@ -356,16 +356,286 @@
     <t>RIK59GUKTV</t>
   </si>
   <si>
-    <t>Expense:</t>
-  </si>
-  <si>
-    <t>Amount (Ksh):</t>
-  </si>
-  <si>
-    <t>Date:</t>
-  </si>
-  <si>
-    <t>Ref:</t>
+    <t>RIL5C4JXNJ</t>
+  </si>
+  <si>
+    <t>RIL4CBCYGE</t>
+  </si>
+  <si>
+    <t>RIN7JSTR7R</t>
+  </si>
+  <si>
+    <t>RIP5OJW4AV</t>
+  </si>
+  <si>
+    <t>RIP8ONL13G</t>
+  </si>
+  <si>
+    <t>RIP5OR2OUD</t>
+  </si>
+  <si>
+    <t>RIP6PS1Y08</t>
+  </si>
+  <si>
+    <t>RIQ4R11F2I</t>
+  </si>
+  <si>
+    <t>RIQ6RHGHZO</t>
+  </si>
+  <si>
+    <t>RIQ8RHW8HW</t>
+  </si>
+  <si>
+    <t>RIQ8RIQCUU</t>
+  </si>
+  <si>
+    <t>RIQ1RPIPB5</t>
+  </si>
+  <si>
+    <t>RIQ2S9XW8C</t>
+  </si>
+  <si>
+    <t>RIQ1SAD08H</t>
+  </si>
+  <si>
+    <t>RIQ0SOBRE6</t>
+  </si>
+  <si>
+    <t>RIQ5SPF8V3</t>
+  </si>
+  <si>
+    <t>RIQ6SS38S6</t>
+  </si>
+  <si>
+    <t>RIQ2T2SMCE</t>
+  </si>
+  <si>
+    <t>RIR7U959EP</t>
+  </si>
+  <si>
+    <t>RIR4UX433G</t>
+  </si>
+  <si>
+    <t>RIS3XH61YH</t>
+  </si>
+  <si>
+    <t>RIS8XSTJNQ</t>
+  </si>
+  <si>
+    <t>RIT91ILILZ</t>
+  </si>
+  <si>
+    <t>RIT01K28GI</t>
+  </si>
+  <si>
+    <t>Gift (church)</t>
+  </si>
+  <si>
+    <t>RJ188QON9I</t>
+  </si>
+  <si>
+    <t>RJ22BMQYNQ</t>
+  </si>
+  <si>
+    <t>RJ29BXLI3D</t>
+  </si>
+  <si>
+    <t>RJ26C4L2UM</t>
+  </si>
+  <si>
+    <t>RJ22CHNRZI</t>
+  </si>
+  <si>
+    <t>Accommodation</t>
+  </si>
+  <si>
+    <t>RJ22CV69PE</t>
+  </si>
+  <si>
+    <t>RJ28E2NNQA</t>
+  </si>
+  <si>
+    <t>Subscription (Netflix)</t>
+  </si>
+  <si>
+    <t>RJ23E6A33R</t>
+  </si>
+  <si>
+    <t>Transport (boda)</t>
+  </si>
+  <si>
+    <t>RJ37EN9U7T</t>
+  </si>
+  <si>
+    <t>RJ31F1NN9P</t>
+  </si>
+  <si>
+    <t>RJ33F23ZQ7</t>
+  </si>
+  <si>
+    <t>RJ38F2U2R2</t>
+  </si>
+  <si>
+    <t>RJ38F3IU4S</t>
+  </si>
+  <si>
+    <t>RJ32FHFSD4</t>
+  </si>
+  <si>
+    <t>RJ38GBC8H4</t>
+  </si>
+  <si>
+    <t>RJ34GE9TLK</t>
+  </si>
+  <si>
+    <t>Purchase (mini 2 propellers)</t>
+  </si>
+  <si>
+    <t>RJ38GKVUZ6</t>
+  </si>
+  <si>
+    <t>RJ39GPUS5F</t>
+  </si>
+  <si>
+    <t>RJ32GV6EP0</t>
+  </si>
+  <si>
+    <t>RJ40I34TWY</t>
+  </si>
+  <si>
+    <t>RJ44I3QGGU</t>
+  </si>
+  <si>
+    <t>RJ46IQJ77Y</t>
+  </si>
+  <si>
+    <t>RJ42JY6RV0</t>
+  </si>
+  <si>
+    <t>RJ51LEZBXH</t>
+  </si>
+  <si>
+    <t>RJ50LF8SXA</t>
+  </si>
+  <si>
+    <t>Transport (tuk tuk)</t>
+  </si>
+  <si>
+    <t>RJ51LK3XH7</t>
+  </si>
+  <si>
+    <t>RJ59LLDIR9</t>
+  </si>
+  <si>
+    <t>RJ55NDDRF9</t>
+  </si>
+  <si>
+    <t>RJ57NKRN3L</t>
+  </si>
+  <si>
+    <t>RJ51NMUSNZ</t>
+  </si>
+  <si>
+    <t>Transport (taxi)</t>
+  </si>
+  <si>
+    <t>RJ57O40X7J</t>
+  </si>
+  <si>
+    <t>RJ65ORQ46D</t>
+  </si>
+  <si>
+    <t>RJ64OSP6CE</t>
+  </si>
+  <si>
+    <t>RJ66OXPFE0</t>
+  </si>
+  <si>
+    <t>RJ66PKME7S</t>
+  </si>
+  <si>
+    <t>RJ61POPBSX</t>
+  </si>
+  <si>
+    <t>RJ63PUWI71</t>
+  </si>
+  <si>
+    <t>RJ63PZPHHJ</t>
+  </si>
+  <si>
+    <t>RJ65Q8KQFF</t>
+  </si>
+  <si>
+    <t>RJ79SRQJVX</t>
+  </si>
+  <si>
+    <t>RJ79U5032T</t>
+  </si>
+  <si>
+    <t>Parking</t>
+  </si>
+  <si>
+    <t>RJ75U8AZYD</t>
+  </si>
+  <si>
+    <t>RJ97YYIFSD</t>
+  </si>
+  <si>
+    <t>RJ93Z0A17F</t>
+  </si>
+  <si>
+    <t>RJ95ZEP7EP</t>
+  </si>
+  <si>
+    <t>RJ92ZKT5I0</t>
+  </si>
+  <si>
+    <t>RJA331E3GL</t>
+  </si>
+  <si>
+    <t>RJA63F3UAU</t>
+  </si>
+  <si>
+    <t>RJA53FJ2WT</t>
+  </si>
+  <si>
+    <t>RJA43KEBX8</t>
+  </si>
+  <si>
+    <t>RJA83QEQUO</t>
+  </si>
+  <si>
+    <t>RJA74DFBVN</t>
+  </si>
+  <si>
+    <t>RJA84EJXGM</t>
+  </si>
+  <si>
+    <t>RJB669U984</t>
+  </si>
+  <si>
+    <t>RJB1700DHJ</t>
+  </si>
+  <si>
+    <t>RJB17FIY8J</t>
+  </si>
+  <si>
+    <t>RJC59HHELH</t>
+  </si>
+  <si>
+    <t>RJC79JMIQN</t>
+  </si>
+  <si>
+    <t>RJC39LN03R</t>
+  </si>
+  <si>
+    <t>RJC0BBR2FE</t>
+  </si>
+  <si>
+    <t>RJC7BEA593</t>
+  </si>
+  <si>
+    <t>RJC8BP987I</t>
   </si>
 </sst>
 </file>
@@ -375,7 +645,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd&quot;/&quot;mm&quot;/&quot;yyyy"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -391,6 +661,10 @@
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -413,7 +687,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -425,6 +699,17 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1945,6 +2230,348 @@
         <v>113</v>
       </c>
     </row>
+    <row r="93">
+      <c r="A93" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B93" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="C93" s="2">
+        <v>45190.0</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B94" s="1">
+        <v>211.0</v>
+      </c>
+      <c r="C94" s="2">
+        <v>45190.0</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B95" s="1">
+        <v>343.0</v>
+      </c>
+      <c r="C95" s="2">
+        <v>45192.0</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B96" s="1">
+        <v>195.0</v>
+      </c>
+      <c r="C96" s="2">
+        <v>45194.0</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B97" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="C97" s="2">
+        <v>45194.0</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B98" s="1">
+        <v>700.0</v>
+      </c>
+      <c r="C98" s="2">
+        <v>45194.0</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B99" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="C99" s="2">
+        <v>45194.0</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B100" s="1">
+        <v>200.0</v>
+      </c>
+      <c r="C100" s="2">
+        <v>45195.0</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B101" s="1">
+        <v>200.0</v>
+      </c>
+      <c r="C101" s="2">
+        <v>45195.0</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B102" s="1">
+        <v>400.0</v>
+      </c>
+      <c r="C102" s="2">
+        <v>45195.0</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B103" s="1">
+        <v>700.0</v>
+      </c>
+      <c r="C103" s="2">
+        <v>45195.0</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B104" s="1">
+        <v>200.0</v>
+      </c>
+      <c r="C104" s="2">
+        <v>45195.0</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B105" s="1">
+        <v>200.0</v>
+      </c>
+      <c r="C105" s="2">
+        <v>45195.0</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B106" s="1">
+        <v>700.0</v>
+      </c>
+      <c r="C106" s="2">
+        <v>45195.0</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B107" s="1">
+        <v>20.0</v>
+      </c>
+      <c r="C107" s="2">
+        <v>45195.0</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B108" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="C108" s="2">
+        <v>45195.0</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B109" s="1">
+        <v>20.0</v>
+      </c>
+      <c r="C109" s="2">
+        <v>45195.0</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B110" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="C110" s="2">
+        <v>45195.0</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B111" s="1">
+        <v>850.0</v>
+      </c>
+      <c r="C111" s="2">
+        <v>45196.0</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B112" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C112" s="2">
+        <v>45196.0</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B113" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="C113" s="2">
+        <v>45197.0</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B114" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="C114" s="2">
+        <v>45197.0</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B115" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="C115" s="2">
+        <v>45198.0</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B116" s="1">
+        <v>120.0</v>
+      </c>
+      <c r="C116" s="2">
+        <v>45198.0</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="C117" s="2"/>
+    </row>
+    <row r="118">
+      <c r="C118" s="2"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C8">
     <cfRule type="timePeriod" dxfId="0" priority="1" timePeriod="today"/>
@@ -1965,16 +2592,884 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>115</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>116</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>117</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1000.0</v>
+      </c>
+      <c r="C2" s="5">
+        <v>45200.0</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="4">
+        <v>300.0</v>
+      </c>
+      <c r="C3" s="5">
+        <v>45201.0</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>45201.0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1">
+        <v>700.0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>45201.0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1">
+        <v>60.0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>45201.0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" s="1">
+        <v>8000.0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>45201.0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>45201.0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B9" s="1">
+        <v>724.0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>45201.0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10" s="1">
+        <v>200.0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>45202.0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B11" s="1">
+        <v>200.0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>45202.0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1">
+        <v>350.0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>45202.0</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1">
+        <v>350.0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>45202.0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B14" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>45202.0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="C15" s="2">
+        <v>45202.0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B16" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="C16" s="2">
+        <v>45202.0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="1">
+        <v>200.0</v>
+      </c>
+      <c r="C17" s="2">
+        <v>45202.0</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B18" s="1">
+        <v>4000.0</v>
+      </c>
+      <c r="C18" s="2">
+        <v>45202.0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>20.0</v>
+      </c>
+      <c r="C19" s="2">
+        <v>45202.0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="C20" s="2">
+        <v>45202.0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="1">
+        <v>850.0</v>
+      </c>
+      <c r="C21" s="2">
+        <v>45203.0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="1">
+        <v>150.0</v>
+      </c>
+      <c r="C22" s="2">
+        <v>45203.0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C23" s="2">
+        <v>45203.0</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B24" s="1">
+        <v>600.0</v>
+      </c>
+      <c r="C24" s="2">
+        <v>45203.0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="C25" s="2">
+        <v>45204.0</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="C26" s="2">
+        <v>45204.0</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B27" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="C27" s="2">
+        <v>45204.0</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B28" s="1">
+        <v>20.0</v>
+      </c>
+      <c r="C28" s="2">
+        <v>45204.0</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="C29" s="2">
+        <v>45204.0</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B30" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="C30" s="2">
+        <v>45204.0</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="C31" s="2">
+        <v>45204.0</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B32" s="1">
+        <v>660.0</v>
+      </c>
+      <c r="C32" s="2">
+        <v>45204.0</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B33" s="1">
+        <v>60.0</v>
+      </c>
+      <c r="C33" s="2">
+        <v>45205.0</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="1">
+        <v>140.0</v>
+      </c>
+      <c r="C34" s="2">
+        <v>45205.0</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B35" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="C35" s="2">
+        <v>45205.0</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B36" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="C36" s="2">
+        <v>45205.0</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="C37" s="2">
+        <v>45205.0</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="1">
+        <v>500.0</v>
+      </c>
+      <c r="C38" s="2">
+        <v>45205.0</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="C39" s="2">
+        <v>45205.0</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" s="1">
+        <v>423.0</v>
+      </c>
+      <c r="C40" s="2">
+        <v>45205.0</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B41" s="1">
+        <v>338.0</v>
+      </c>
+      <c r="C41" s="2">
+        <v>45206.0</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" s="1">
+        <v>279.0</v>
+      </c>
+      <c r="C42" s="2">
+        <v>45206.0</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B43" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="C43" s="2">
+        <v>45206.0</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" s="4">
+        <v>300.0</v>
+      </c>
+      <c r="C44" s="2">
+        <v>45208.0</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" s="1">
+        <v>219.0</v>
+      </c>
+      <c r="C45" s="2">
+        <v>45208.0</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="C46" s="2">
+        <v>45208.0</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" s="1">
+        <v>700.0</v>
+      </c>
+      <c r="C47" s="2">
+        <v>45208.0</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B48" s="1">
+        <v>200.0</v>
+      </c>
+      <c r="C48" s="2">
+        <v>45209.0</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B49" s="1">
+        <v>300.0</v>
+      </c>
+      <c r="C49" s="2">
+        <v>45209.0</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B50" s="1">
+        <v>350.0</v>
+      </c>
+      <c r="C50" s="2">
+        <v>45209.0</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" s="1">
+        <v>400.0</v>
+      </c>
+      <c r="C51" s="2">
+        <v>45209.0</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B52" s="7">
+        <v>100.0</v>
+      </c>
+      <c r="C52" s="8">
+        <v>45209.0</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B53" s="7">
+        <v>100.0</v>
+      </c>
+      <c r="C53" s="8">
+        <v>45209.0</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="1">
+        <v>300.0</v>
+      </c>
+      <c r="C54" s="2">
+        <v>45209.0</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" s="1">
+        <v>750.0</v>
+      </c>
+      <c r="C55" s="2">
+        <v>45210.0</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C56" s="2">
+        <v>45210.0</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B57" s="1">
+        <v>268.0</v>
+      </c>
+      <c r="C57" s="2">
+        <v>45210.0</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="C58" s="2">
+        <v>45211.0</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1000.0</v>
+      </c>
+      <c r="C59" s="2">
+        <v>45211.0</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B60" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="C60" s="2">
+        <v>45211.0</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B61" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="C61" s="2">
+        <v>45211.0</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B62" s="1">
+        <v>60.0</v>
+      </c>
+      <c r="C62" s="2">
+        <v>45211.0</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B63" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="C63" s="2">
+        <v>45211.0</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>